<commit_message>
adds y/n indication for dCas9 design
</commit_message>
<xml_diff>
--- a/gRNA_target_design/Benchling_final_gRNA.xlsx
+++ b/gRNA_target_design/Benchling_final_gRNA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="5595" yWindow="-30" windowWidth="16320" windowHeight="5910"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="MASTER Target Candidates" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="154">
   <si>
     <t>Scenario</t>
   </si>
@@ -486,11 +486,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,7 +1091,27 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1300,7 +1320,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1335,7 +1354,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1511,14 +1529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -1537,7 +1555,7 @@
     <col min="17" max="17" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
@@ -1612,7 +1630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="50" t="s">
         <v>19</v>
       </c>
@@ -1642,7 +1660,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="50" t="s">
         <v>22</v>
       </c>
@@ -1671,7 +1689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="M6" s="83" t="s">
         <v>26</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="M7" t="s">
         <v>27</v>
       </c>
@@ -1706,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="83" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1745,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="82" t="s">
         <v>29</v>
       </c>
@@ -1779,7 +1797,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="28">
         <v>1</v>
       </c>
@@ -1832,7 +1850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -1885,7 +1903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -1938,7 +1956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -1992,7 +2010,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -2046,7 +2064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="29">
         <v>6</v>
       </c>
@@ -2086,7 +2104,7 @@
       <c r="M15" s="83"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="29">
         <v>7</v>
       </c>
@@ -2127,7 +2145,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="29">
         <v>8</v>
       </c>
@@ -2168,7 +2186,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="29">
         <v>9</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="29">
         <v>10</v>
       </c>
@@ -2250,7 +2268,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="29">
         <v>11</v>
       </c>
@@ -2288,7 +2306,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="29">
         <v>12</v>
       </c>
@@ -2326,7 +2344,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="29">
         <v>13</v>
       </c>
@@ -2361,7 +2379,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="29">
         <v>14</v>
       </c>
@@ -2396,7 +2414,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="29">
         <v>15</v>
       </c>
@@ -2431,7 +2449,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="29">
         <v>16</v>
       </c>
@@ -2466,7 +2484,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="29">
         <v>17</v>
       </c>
@@ -2501,7 +2519,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="29">
         <v>18</v>
       </c>
@@ -2536,7 +2554,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="29">
         <v>19</v>
       </c>
@@ -2571,7 +2589,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="30">
         <v>20</v>
       </c>
@@ -2606,7 +2624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="52"/>
@@ -2619,18 +2637,18 @@
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="83" t="s">
         <v>13</v>
       </c>
       <c r="L32" s="83"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="82" t="s">
         <v>29</v>
       </c>
@@ -2674,7 +2692,7 @@
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" s="28">
         <v>1</v>
       </c>
@@ -2718,7 +2736,7 @@
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" s="29">
         <v>2</v>
       </c>
@@ -2762,7 +2780,7 @@
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23">
       <c r="A36" s="71">
         <v>3</v>
       </c>
@@ -2808,7 +2826,7 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23">
       <c r="A37" s="71">
         <v>4</v>
       </c>
@@ -2854,7 +2872,7 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" s="71">
         <v>5</v>
       </c>
@@ -2900,7 +2918,7 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23">
       <c r="A39" s="71">
         <v>6</v>
       </c>
@@ -2946,7 +2964,7 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23">
       <c r="A40" s="71">
         <v>7</v>
       </c>
@@ -2990,7 +3008,7 @@
       <c r="T40" s="5"/>
       <c r="U40" s="14"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23">
       <c r="A41" s="71">
         <v>8</v>
       </c>
@@ -3034,7 +3052,7 @@
       <c r="T41" s="5"/>
       <c r="U41" s="14"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23">
       <c r="A42" s="71">
         <v>9</v>
       </c>
@@ -3078,7 +3096,7 @@
       <c r="T42" s="5"/>
       <c r="U42" s="14"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23">
       <c r="A43" s="71">
         <v>10</v>
       </c>
@@ -3122,7 +3140,7 @@
       <c r="T43" s="5"/>
       <c r="U43" s="14"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23">
       <c r="A44" s="65">
         <v>11</v>
       </c>
@@ -3166,7 +3184,7 @@
       <c r="T44" s="5"/>
       <c r="U44" s="14"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="L45" s="83"/>
@@ -3179,7 +3197,7 @@
       <c r="T45" s="5"/>
       <c r="U45" s="14"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23">
       <c r="A46" s="83" t="s">
         <v>19</v>
       </c>
@@ -3193,7 +3211,7 @@
       <c r="T46" s="5"/>
       <c r="U46" s="14"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23">
       <c r="A47" s="82" t="s">
         <v>29</v>
       </c>
@@ -3237,7 +3255,7 @@
       <c r="T47" s="5"/>
       <c r="U47" s="14"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23">
       <c r="A48" s="28">
         <v>1</v>
       </c>
@@ -3281,7 +3299,7 @@
       <c r="T48" s="5"/>
       <c r="U48" s="14"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21">
       <c r="A49" s="29">
         <v>2</v>
       </c>
@@ -3325,7 +3343,7 @@
       <c r="T49" s="5"/>
       <c r="U49" s="14"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21">
       <c r="A50" s="29">
         <v>3</v>
       </c>
@@ -3369,7 +3387,7 @@
       <c r="T50" s="5"/>
       <c r="U50" s="14"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21">
       <c r="A51" s="29">
         <v>4</v>
       </c>
@@ -3413,7 +3431,7 @@
       <c r="T51" s="5"/>
       <c r="U51" s="14"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21">
       <c r="A52" s="29">
         <v>5</v>
       </c>
@@ -3455,7 +3473,7 @@
       <c r="T52" s="13"/>
       <c r="U52" s="14"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21">
       <c r="A53" s="29">
         <v>6</v>
       </c>
@@ -3497,7 +3515,7 @@
       <c r="T53" s="5"/>
       <c r="U53" s="14"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21">
       <c r="A54" s="29">
         <v>7</v>
       </c>
@@ -3539,7 +3557,7 @@
       <c r="T54" s="5"/>
       <c r="U54" s="14"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21">
       <c r="A55" s="29">
         <v>8</v>
       </c>
@@ -3581,7 +3599,7 @@
       <c r="T55" s="5"/>
       <c r="U55" s="14"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21">
       <c r="A56" s="30">
         <v>9</v>
       </c>
@@ -3624,7 +3642,7 @@
       <c r="T56" s="5"/>
       <c r="U56" s="14"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="1"/>
@@ -3647,7 +3665,7 @@
       <c r="T57" s="5"/>
       <c r="U57" s="14"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21">
       <c r="A58" s="83" t="s">
         <v>22</v>
       </c>
@@ -3662,7 +3680,7 @@
       <c r="T58" s="13"/>
       <c r="U58" s="13"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21">
       <c r="A59" s="82" t="s">
         <v>29</v>
       </c>
@@ -3707,7 +3725,7 @@
       <c r="T59" s="13"/>
       <c r="U59" s="13"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21">
       <c r="A60" s="29">
         <v>1</v>
       </c>
@@ -3735,7 +3753,9 @@
       <c r="I60" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J60" s="13"/>
+      <c r="J60" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K60" s="19"/>
       <c r="M60" s="9"/>
       <c r="N60" s="13"/>
@@ -3747,7 +3767,7 @@
       <c r="T60" s="13"/>
       <c r="U60" s="13"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21">
       <c r="A61" s="29">
         <v>2</v>
       </c>
@@ -3775,7 +3795,9 @@
       <c r="I61" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J61" s="13"/>
+      <c r="J61" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="K61" s="19"/>
       <c r="M61" s="9"/>
       <c r="N61" s="13"/>
@@ -3787,7 +3809,7 @@
       <c r="T61" s="13"/>
       <c r="U61" s="13"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21">
       <c r="A62" s="29">
         <v>3</v>
       </c>
@@ -3815,14 +3837,16 @@
       <c r="I62" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J62" s="13"/>
+      <c r="J62" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="K62" s="19"/>
       <c r="M62" s="9"/>
       <c r="N62" s="13"/>
       <c r="O62" s="13"/>
       <c r="P62" s="13"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21">
       <c r="A63" s="29">
         <v>4</v>
       </c>
@@ -3850,14 +3874,16 @@
       <c r="I63" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J63" s="13"/>
+      <c r="J63" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="K63" s="19"/>
       <c r="M63" s="94"/>
       <c r="N63" s="13"/>
       <c r="O63" s="13"/>
       <c r="P63" s="13"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21">
       <c r="A64" s="29">
         <v>5</v>
       </c>
@@ -3885,14 +3911,16 @@
       <c r="I64" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J64" s="13"/>
+      <c r="J64" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="K64" s="19"/>
       <c r="M64" s="9"/>
       <c r="N64" s="13"/>
       <c r="O64" s="13"/>
       <c r="P64" s="13"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19">
       <c r="A65" s="29">
         <v>6</v>
       </c>
@@ -3920,14 +3948,16 @@
       <c r="I65" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J65" s="13"/>
+      <c r="J65" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="K65" s="19"/>
       <c r="M65" s="9"/>
       <c r="N65" s="13"/>
       <c r="O65" s="13"/>
       <c r="P65" s="13"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19">
       <c r="A66" s="30">
         <v>7</v>
       </c>
@@ -3955,14 +3985,16 @@
       <c r="I66" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J66" s="17"/>
+      <c r="J66" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="K66" s="26"/>
       <c r="M66" s="13"/>
       <c r="N66" s="13"/>
       <c r="O66" s="13"/>
       <c r="P66" s="13"/>
     </row>
-    <row r="67" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="15.75">
       <c r="A67" s="29">
         <v>8</v>
       </c>
@@ -3990,7 +4022,9 @@
       <c r="I67" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="18"/>
+      <c r="J67" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="K67" s="22"/>
       <c r="M67" s="13"/>
       <c r="N67" s="9"/>
@@ -4000,7 +4034,7 @@
       <c r="R67" s="6"/>
       <c r="S67" s="5"/>
     </row>
-    <row r="68" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="15.75">
       <c r="A68" s="34"/>
       <c r="B68" s="95"/>
       <c r="C68" s="18"/>
@@ -4020,7 +4054,7 @@
       <c r="R68" s="6"/>
       <c r="S68" s="5"/>
     </row>
-    <row r="69" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="15.75">
       <c r="A69" s="8"/>
       <c r="B69" s="9"/>
       <c r="C69" s="13"/>
@@ -4040,7 +4074,7 @@
       <c r="R69" s="6"/>
       <c r="S69" s="5"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
       <c r="C70" s="13"/>
@@ -4057,7 +4091,7 @@
       <c r="O70" s="13"/>
       <c r="P70" s="13"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19">
       <c r="A71" s="8"/>
       <c r="B71" s="9"/>
       <c r="C71" s="13"/>
@@ -4074,7 +4108,7 @@
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
       <c r="C72" s="13"/>
@@ -4091,7 +4125,7 @@
       <c r="O72" s="13"/>
       <c r="P72" s="13"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19">
       <c r="A73" s="8"/>
       <c r="B73" s="9"/>
       <c r="C73" s="13"/>
@@ -4108,7 +4142,7 @@
       <c r="O73" s="13"/>
       <c r="P73" s="13"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19">
       <c r="A74" s="8"/>
       <c r="B74" s="9"/>
       <c r="C74" s="13"/>
@@ -4121,7 +4155,7 @@
       <c r="J74" s="13"/>
       <c r="K74" s="13"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19">
       <c r="A75" s="13"/>
       <c r="B75" s="9"/>
       <c r="C75" s="13"/>
@@ -4136,47 +4170,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J9:J33 J38:J42 J45:J47 J52:J66">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:J37">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:J44">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:J51">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J60:J67">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>